<commit_message>
Optional constant names added to file input
</commit_message>
<xml_diff>
--- a/input/dsl.3/data.input.xlsx
+++ b/input/dsl.3/data.input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\dsl.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03EB14C-53FF-4956-BCC6-54B377CBC6F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CC1394-24C2-455F-A6C8-6CB831699134}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="k_constants_log10" sheetId="3" r:id="rId3"/>
     <sheet name="absorbance" sheetId="4" r:id="rId4"/>
     <sheet name="mol_ext_coefficients" sheetId="5" r:id="rId5"/>
+    <sheet name="constant_names" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>H</t>
   </si>
@@ -1330,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EF57C8-A1DB-4B5D-9903-403F1593211A}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1348,4 +1349,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D11D97-DC3D-468C-BFC1-901C7148BABC}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working with no known molar extinction coefficients
</commit_message>
<xml_diff>
--- a/input/dsl.3/data.input.xlsx
+++ b/input/dsl.3/data.input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\dsl.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CC1394-24C2-455F-A6C8-6CB831699134}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D439A98-687B-4040-AF2E-F0755F32A8CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -1331,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EF57C8-A1DB-4B5D-9903-403F1593211A}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1355,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D11D97-DC3D-468C-BFC1-901C7148BABC}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>